<commit_message>
filled digikey mpn and inventory:
</commit_message>
<xml_diff>
--- a/bom/actuation.xlsx
+++ b/bom/actuation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameron/Dropbox/Development/actuation-pcb/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherxu/KiCad/actuation-pcb/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C1B714BD-7A5C-B148-9A59-2390202C07E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969E15AE-897A-0A4F-BEAB-1764EF2AEF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actuation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="312">
   <si>
     <t>Reference</t>
   </si>
@@ -695,13 +695,274 @@
   </si>
   <si>
     <t>Digi-Key P/N</t>
+  </si>
+  <si>
+    <t>490-3285-1-ND</t>
+  </si>
+  <si>
+    <t>490-12330-1-ND</t>
+  </si>
+  <si>
+    <t>1276-3388-1-ND</t>
+  </si>
+  <si>
+    <t>490-5777-1-ND</t>
+  </si>
+  <si>
+    <t>490-11477-1-ND</t>
+  </si>
+  <si>
+    <t>1276-6767-1-ND</t>
+  </si>
+  <si>
+    <t>490-GRT1885C1E103JA02JCT-ND</t>
+  </si>
+  <si>
+    <t>490-6385-1-ND</t>
+  </si>
+  <si>
+    <t>490-5799-1-ND</t>
+  </si>
+  <si>
+    <t>490-5309-1-ND</t>
+  </si>
+  <si>
+    <t>490-10516-1-ND</t>
+  </si>
+  <si>
+    <t>1727-3833-1-ND</t>
+  </si>
+  <si>
+    <t>1727-3825-1-ND</t>
+  </si>
+  <si>
+    <t>B2100A-13-FDICT-ND</t>
+  </si>
+  <si>
+    <t>160-1445-1-ND</t>
+  </si>
+  <si>
+    <t>160-1446-1-ND</t>
+  </si>
+  <si>
+    <t>160-1447-1-ND</t>
+  </si>
+  <si>
+    <t>160-1647-1-ND</t>
+  </si>
+  <si>
+    <t>SMAJ40CA-FDICT-ND</t>
+  </si>
+  <si>
+    <t>160-2239-1-ND</t>
+  </si>
+  <si>
+    <t>SMAJ28CAQ-13-FDICT-ND</t>
+  </si>
+  <si>
+    <t>182-109FE-ND</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>enough</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>277-1578-ND</t>
+  </si>
+  <si>
+    <t>277-1667-ND</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>2449-J115F11CH12VDCSH1.5U-ND</t>
+  </si>
+  <si>
+    <t>541-1238-1-ND</t>
+  </si>
+  <si>
+    <t>SI7220DN-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t>1727-1900-1-ND</t>
+  </si>
+  <si>
+    <t>311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t>311-120HRCT-ND</t>
+  </si>
+  <si>
+    <t>YAG1238CT-ND</t>
+  </si>
+  <si>
+    <t>311-270HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-470HRCT-ND</t>
+  </si>
+  <si>
+    <t>311-2592-1-ND</t>
+  </si>
+  <si>
+    <t>311-2107-1-ND</t>
+  </si>
+  <si>
+    <t>311-2395-1-ND</t>
+  </si>
+  <si>
+    <t>311-2422-1-ND</t>
+  </si>
+  <si>
+    <t>13-RC0603FR-071M87LCT-ND</t>
+  </si>
+  <si>
+    <t>YAG1636CT-ND</t>
+  </si>
+  <si>
+    <t>311-510KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-10.0HRCT-ND</t>
+  </si>
+  <si>
+    <t>YAG3621CT-ND</t>
+  </si>
+  <si>
+    <t>YAG3575CT-ND</t>
+  </si>
+  <si>
+    <t>311-10.0KHRCT-ND</t>
+  </si>
+  <si>
+    <t>311-2691-1-ND</t>
+  </si>
+  <si>
+    <t>311-69.8KDCT-ND</t>
+  </si>
+  <si>
+    <t>YAG1590CT-ND</t>
+  </si>
+  <si>
+    <t>311-1.00KHRCT-ND</t>
+  </si>
+  <si>
+    <t>3224W-103ECT-ND</t>
+  </si>
+  <si>
+    <t>568-PCA9615DPZCT-ND</t>
+  </si>
+  <si>
+    <t>TI sample?</t>
+  </si>
+  <si>
+    <t>out of stock :(</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>DSUB</t>
+  </si>
+  <si>
+    <t>TLP241A(TP1FCT-ND</t>
+  </si>
+  <si>
+    <t>296-21764-1-ND</t>
+  </si>
+  <si>
+    <t>TLP2366(V4-TPLECT-ND</t>
+  </si>
+  <si>
+    <t>296-TLV7031QDCKRQ1CT-ND</t>
+  </si>
+  <si>
+    <t>1727-6066-1-ND</t>
+  </si>
+  <si>
+    <t>296-8521-1-ND</t>
+  </si>
+  <si>
+    <t>505-LTC4367IDD-1#PBF-ND</t>
+  </si>
+  <si>
+    <t>296-14462-1-ND</t>
+  </si>
+  <si>
+    <t>out of stock :( Analog sample?</t>
+  </si>
+  <si>
+    <t>31-AP64350SP-13CT-ND</t>
+  </si>
+  <si>
+    <t>296-47214-1-ND</t>
+  </si>
+  <si>
+    <t>Order Qty</t>
+  </si>
+  <si>
+    <t>inventory rated for 50V</t>
+  </si>
+  <si>
+    <t>inventory rated for 25V</t>
+  </si>
+  <si>
+    <t>inventory rated for 10V</t>
+  </si>
+  <si>
+    <t>white led</t>
+  </si>
+  <si>
+    <t>orange led</t>
+  </si>
+  <si>
+    <t>blue led</t>
+  </si>
+  <si>
+    <t>have 3 of LTST-C190TGKT</t>
+  </si>
+  <si>
+    <t>red led</t>
+  </si>
+  <si>
+    <t>LCSC, 10 each of C98733 and C129184</t>
+  </si>
+  <si>
+    <t>big relay</t>
+  </si>
+  <si>
+    <t>1.87M 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>32.4k 0.1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>510k 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>10 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>5.1k 0.1% 1/10W 0.603</t>
+  </si>
+  <si>
+    <t>10k 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>1k 1% 1/10W 0603</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -832,6 +1093,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1134,7 +1403,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1177,12 +1446,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1216,6 +1488,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1535,22 +1808,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1569,8 +1846,17 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H1" t="s">
+        <v>294</v>
+      </c>
+      <c r="I1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1583,11 +1869,17 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="F2">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1600,11 +1892,20 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="F3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1617,11 +1918,17 @@
       <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>227</v>
+      </c>
       <c r="F4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1634,11 +1941,17 @@
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1651,11 +1964,17 @@
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>229</v>
+      </c>
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1668,11 +1987,20 @@
       <c r="D7" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="F7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="I7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1685,11 +2013,20 @@
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>90</v>
+      </c>
+      <c r="I8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1702,11 +2039,17 @@
       <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1719,11 +2062,17 @@
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1736,11 +2085,20 @@
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="F11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1753,11 +2111,20 @@
       <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="E12" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="F12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>80</v>
+      </c>
+      <c r="I12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1770,11 +2137,17 @@
       <c r="D13" s="1" t="s">
         <v>41</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1787,11 +2160,17 @@
       <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>237</v>
+      </c>
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1804,11 +2183,17 @@
       <c r="D15" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="E15" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="F15">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -1821,11 +2206,20 @@
       <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="E16" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="F16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>211</v>
       </c>
@@ -1838,11 +2232,20 @@
       <c r="D17" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="E17" s="1" t="s">
+        <v>240</v>
+      </c>
       <c r="F17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>213</v>
       </c>
@@ -1855,11 +2258,20 @@
       <c r="D18" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="F18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>210</v>
       </c>
@@ -1872,11 +2284,20 @@
       <c r="D19" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E19" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="F19">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1889,11 +2310,17 @@
       <c r="D20" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1906,11 +2333,20 @@
       <c r="D21" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1923,11 +2359,17 @@
       <c r="D22" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -1940,11 +2382,20 @@
       <c r="D23" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>248</v>
+      </c>
+      <c r="I23" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -1957,11 +2408,20 @@
       <c r="D24" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="E24" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="F24">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>30</v>
+      </c>
+      <c r="I24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>216</v>
       </c>
@@ -1974,11 +2434,17 @@
       <c r="D25" s="1">
         <v>1935174</v>
       </c>
+      <c r="E25" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="F25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>218</v>
       </c>
@@ -1991,11 +2457,17 @@
       <c r="D26" s="1">
         <v>1935161</v>
       </c>
+      <c r="E26" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="F26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>221</v>
       </c>
@@ -2008,11 +2480,20 @@
       <c r="D27" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="E27" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="F27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>223</v>
       </c>
@@ -2025,11 +2506,20 @@
       <c r="D28" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="E28" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="F28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>20</v>
+      </c>
+      <c r="I28" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -2042,11 +2532,20 @@
       <c r="D29" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="E29" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2059,11 +2558,17 @@
       <c r="D30" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="E30" s="1" t="s">
+        <v>254</v>
+      </c>
       <c r="F30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -2076,11 +2581,17 @@
       <c r="D31" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="E31" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="F31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -2093,11 +2604,17 @@
       <c r="D32" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="E32" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>88</v>
       </c>
@@ -2110,11 +2627,17 @@
       <c r="D33" s="1" t="s">
         <v>91</v>
       </c>
+      <c r="E33" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -2127,11 +2650,17 @@
       <c r="D34" s="1" t="s">
         <v>94</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2144,11 +2673,17 @@
       <c r="D35" s="1" t="s">
         <v>97</v>
       </c>
+      <c r="E35" s="1" t="s">
+        <v>258</v>
+      </c>
       <c r="F35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>98</v>
       </c>
@@ -2161,11 +2696,17 @@
       <c r="D36" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>259</v>
+      </c>
       <c r="F36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -2178,11 +2719,17 @@
       <c r="D37" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>260</v>
+      </c>
       <c r="F37">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>104</v>
       </c>
@@ -2195,11 +2742,17 @@
       <c r="D38" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="E38" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="F38">
         <v>27</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -2212,11 +2765,17 @@
       <c r="D39" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="F39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -2229,11 +2788,17 @@
       <c r="D40" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="E40" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="F40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -2246,11 +2811,17 @@
       <c r="D41" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="E41" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="F41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>116</v>
       </c>
@@ -2263,11 +2834,17 @@
       <c r="D42" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="E42" s="1" t="s">
+        <v>265</v>
+      </c>
       <c r="F42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -2280,11 +2857,20 @@
       <c r="D43" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="E43" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>90</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -2297,11 +2883,20 @@
       <c r="D44" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>8</v>
+      </c>
+      <c r="I44" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>125</v>
       </c>
@@ -2314,11 +2909,20 @@
       <c r="D45" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="E45" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>90</v>
+      </c>
+      <c r="I45" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>128</v>
       </c>
@@ -2331,11 +2935,20 @@
       <c r="D46" s="1" t="s">
         <v>130</v>
       </c>
+      <c r="E46" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="F46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46">
+        <v>90</v>
+      </c>
+      <c r="I46" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>131</v>
       </c>
@@ -2348,11 +2961,20 @@
       <c r="D47" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="E47" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="I47" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>134</v>
       </c>
@@ -2365,11 +2987,17 @@
       <c r="D48" s="1" t="s">
         <v>136</v>
       </c>
+      <c r="E48" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>137</v>
       </c>
@@ -2382,11 +3010,20 @@
       <c r="D49" s="1" t="s">
         <v>139</v>
       </c>
+      <c r="E49" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="F49">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49">
+        <v>90</v>
+      </c>
+      <c r="I49" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>140</v>
       </c>
@@ -2399,11 +3036,17 @@
       <c r="D50" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="F50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>143</v>
       </c>
@@ -2416,11 +3059,17 @@
       <c r="D51" s="1" t="s">
         <v>145</v>
       </c>
+      <c r="E51" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="F51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>146</v>
       </c>
@@ -2433,11 +3082,17 @@
       <c r="D52" s="1" t="s">
         <v>148</v>
       </c>
+      <c r="E52" s="1" t="s">
+        <v>275</v>
+      </c>
       <c r="F52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>149</v>
       </c>
@@ -2450,11 +3105,20 @@
       <c r="D53" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="E53" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="F53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53">
+        <v>85</v>
+      </c>
+      <c r="I53" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>152</v>
       </c>
@@ -2467,11 +3131,17 @@
       <c r="D54" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="E54" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="F54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>155</v>
       </c>
@@ -2484,11 +3154,20 @@
       <c r="D55" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="E55" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="F55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="I55" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>159</v>
       </c>
@@ -2501,11 +3180,20 @@
       <c r="D56" s="1" t="s">
         <v>162</v>
       </c>
+      <c r="E56" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="F56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="I56" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>163</v>
       </c>
@@ -2518,11 +3206,17 @@
       <c r="D57" s="1" t="s">
         <v>166</v>
       </c>
+      <c r="E57" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="F57">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>167</v>
       </c>
@@ -2535,11 +3229,20 @@
       <c r="D58" s="1" t="s">
         <v>170</v>
       </c>
+      <c r="E58" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="F58">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="I58" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>171</v>
       </c>
@@ -2552,11 +3255,17 @@
       <c r="D59" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="E59" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="F59">
         <v>8</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>175</v>
       </c>
@@ -2569,11 +3278,20 @@
       <c r="D60" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="E60" s="1" t="s">
+        <v>286</v>
+      </c>
       <c r="F60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="I60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -2586,11 +3304,17 @@
       <c r="D61" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="E61" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="F61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>183</v>
       </c>
@@ -2603,11 +3327,20 @@
       <c r="D62" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="E62" s="1" t="s">
+        <v>288</v>
+      </c>
       <c r="F62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="I62" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>187</v>
       </c>
@@ -2620,11 +3353,17 @@
       <c r="D63" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="E63" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="F63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>191</v>
       </c>
@@ -2637,11 +3376,20 @@
       <c r="D64" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="E64" s="1" t="s">
+        <v>289</v>
+      </c>
       <c r="F64">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="I64" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>195</v>
       </c>
@@ -2654,11 +3402,20 @@
       <c r="D65" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="E65" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="F65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="I65" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>199</v>
       </c>
@@ -2671,11 +3428,17 @@
       <c r="D66" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="E66" s="1" t="s">
+        <v>292</v>
+      </c>
       <c r="F66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -2688,11 +3451,23 @@
       <c r="D67" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="E67" s="1" t="s">
+        <v>293</v>
+      </c>
       <c r="F67">
         <v>1</v>
       </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="I67" t="s">
+        <v>279</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1" location="gid=0" xr:uid="{41232F66-F9A6-794D-8DA3-D9C3B4CF7D38}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM for ordering
</commit_message>
<xml_diff>
--- a/bom/actuation.xlsx
+++ b/bom/actuation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherxu/KiCad/actuation-pcb/bom/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameron/Dropbox/Development/actuation-pcb/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969E15AE-897A-0A4F-BEAB-1764EF2AEF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B476EAC-ECC3-1F4C-9DB3-7D3B20B7B42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actuation" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="313">
   <si>
     <t>Reference</t>
   </si>
@@ -286,18 +286,9 @@
     <t>PMV40UN2R</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_0603_1608Metric</t>
   </si>
   <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
     <t>R2, R4, R5, R7</t>
   </si>
   <si>
@@ -793,9 +784,6 @@
     <t>1727-1900-1-ND</t>
   </si>
   <si>
-    <t>311-0.0GRCT-ND</t>
-  </si>
-  <si>
     <t>311-120HRCT-ND</t>
   </si>
   <si>
@@ -956,6 +944,21 @@
   </si>
   <si>
     <t>1k 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>448-TLI4971A050T5UE0001XUMA1CT-ND</t>
+  </si>
+  <si>
+    <t>296-43875-1-ND</t>
+  </si>
+  <si>
+    <t>311-604HRCT-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/b8pdp9ph</t>
+  </si>
+  <si>
+    <t>Digi-Key cart</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1286,6 +1289,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1448,11 +1457,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1809,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1821,7 +1831,7 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="9" max="9" width="26.5" customWidth="1"/>
@@ -1841,19 +1851,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="I1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1870,13 +1880,16 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F2">
         <v>25</v>
       </c>
       <c r="G2">
         <v>80</v>
+      </c>
+      <c r="H2">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1893,7 +1906,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -1901,8 +1914,11 @@
       <c r="G3">
         <v>80</v>
       </c>
+      <c r="H3">
+        <v>50</v>
+      </c>
       <c r="I3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1919,13 +1935,16 @@
         <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F4">
         <v>16</v>
       </c>
       <c r="G4">
         <v>4</v>
+      </c>
+      <c r="H4">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1942,13 +1961,16 @@
         <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5">
         <v>90</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1965,13 +1987,16 @@
         <v>21</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6">
         <v>0</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1988,7 +2013,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1996,8 +2021,11 @@
       <c r="G7">
         <v>4</v>
       </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
       <c r="I7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2014,7 +2042,7 @@
         <v>27</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -2022,8 +2050,11 @@
       <c r="G8">
         <v>90</v>
       </c>
+      <c r="H8">
+        <v>10</v>
+      </c>
       <c r="I8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2040,13 +2071,16 @@
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -2063,13 +2097,16 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
         <v>0</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2086,7 +2123,7 @@
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -2094,8 +2131,11 @@
       <c r="G11">
         <v>6</v>
       </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
       <c r="I11" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -2112,7 +2152,7 @@
         <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F12">
         <v>2</v>
@@ -2120,8 +2160,11 @@
       <c r="G12">
         <v>80</v>
       </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
       <c r="I12" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -2138,13 +2181,16 @@
         <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -2161,13 +2207,16 @@
         <v>43</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
         <v>0</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -2184,7 +2233,7 @@
         <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F15">
         <v>17</v>
@@ -2192,13 +2241,16 @@
       <c r="G15">
         <v>8</v>
       </c>
+      <c r="H15">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B16" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
@@ -2207,7 +2259,7 @@
         <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F16">
         <v>16</v>
@@ -2215,16 +2267,19 @@
       <c r="G16">
         <v>0</v>
       </c>
+      <c r="H16">
+        <v>24</v>
+      </c>
       <c r="I16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
@@ -2233,7 +2288,7 @@
         <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -2241,16 +2296,19 @@
       <c r="G17">
         <v>0</v>
       </c>
+      <c r="H17">
+        <v>20</v>
+      </c>
       <c r="I17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C18" t="s">
         <v>48</v>
@@ -2259,7 +2317,7 @@
         <v>51</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F18">
         <v>3</v>
@@ -2267,16 +2325,19 @@
       <c r="G18">
         <v>0</v>
       </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
       <c r="I18" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C19" t="s">
         <v>48</v>
@@ -2285,7 +2346,7 @@
         <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F19">
         <v>6</v>
@@ -2293,8 +2354,11 @@
       <c r="G19">
         <v>8</v>
       </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
       <c r="I19" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -2311,13 +2375,16 @@
         <v>54</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
         <v>3</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -2334,7 +2401,7 @@
         <v>57</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2342,8 +2409,11 @@
       <c r="G21">
         <v>6</v>
       </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
       <c r="I21" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -2360,13 +2430,16 @@
         <v>59</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
         <v>0</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -2383,24 +2456,27 @@
         <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F23">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C24" t="s">
         <v>64</v>
@@ -2409,7 +2485,7 @@
         <v>65</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F24">
         <v>16</v>
@@ -2417,16 +2493,19 @@
       <c r="G24">
         <v>30</v>
       </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
       <c r="I24" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B25" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C25" t="s">
         <v>66</v>
@@ -2435,7 +2514,7 @@
         <v>1935174</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F25">
         <v>3</v>
@@ -2443,13 +2522,16 @@
       <c r="G25">
         <v>0</v>
       </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C26" t="s">
         <v>67</v>
@@ -2458,7 +2540,7 @@
         <v>1935161</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -2466,13 +2548,16 @@
       <c r="G26">
         <v>0</v>
       </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B27" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C27" t="s">
         <v>68</v>
@@ -2481,7 +2566,7 @@
         <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F27">
         <v>2</v>
@@ -2489,16 +2574,19 @@
       <c r="G27">
         <v>4</v>
       </c>
+      <c r="H27" s="4">
+        <v>0</v>
+      </c>
       <c r="I27" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C28" t="s">
         <v>70</v>
@@ -2507,7 +2595,7 @@
         <v>71</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -2515,8 +2603,11 @@
       <c r="G28">
         <v>20</v>
       </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
       <c r="I28" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -2533,7 +2624,7 @@
         <v>75</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2541,8 +2632,11 @@
       <c r="G29">
         <v>1</v>
       </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
       <c r="I29" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2559,13 +2653,16 @@
         <v>79</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
       <c r="G30">
         <v>0</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -2582,13 +2679,16 @@
         <v>83</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F31">
         <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
+      </c>
+      <c r="H31">
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -2605,7 +2705,7 @@
         <v>87</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2613,28 +2713,34 @@
       <c r="G32">
         <v>0</v>
       </c>
+      <c r="H32">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
         <v>88</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>90</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>91</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>257</v>
+        <v>310</v>
       </c>
       <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="I33" t="s">
-        <v>89</v>
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -2645,19 +2751,22 @@
         <v>93</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>94</v>
+        <v>254</v>
       </c>
       <c r="F34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G34">
         <v>0</v>
+      </c>
+      <c r="H34">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -2668,19 +2777,22 @@
         <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G35">
         <v>0</v>
+      </c>
+      <c r="H35">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -2691,19 +2803,22 @@
         <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>100</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="F36">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="G36">
         <v>0</v>
+      </c>
+      <c r="H36">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -2714,19 +2829,22 @@
         <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>103</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F37">
         <v>27</v>
       </c>
       <c r="G37">
         <v>0</v>
+      </c>
+      <c r="H37">
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -2737,19 +2855,22 @@
         <v>105</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>106</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F38">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="G38">
         <v>0</v>
+      </c>
+      <c r="H38">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -2760,19 +2881,22 @@
         <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G39">
         <v>0</v>
+      </c>
+      <c r="H39">
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -2783,19 +2907,22 @@
         <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>112</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G40">
         <v>0</v>
+      </c>
+      <c r="H40">
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -2806,19 +2933,22 @@
         <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>115</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G41">
         <v>0</v>
+      </c>
+      <c r="H41">
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -2829,19 +2959,25 @@
         <v>117</v>
       </c>
       <c r="C42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2852,22 +2988,25 @@
         <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>121</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F43">
         <v>1</v>
       </c>
       <c r="G43">
-        <v>90</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>305</v>
+        <v>8</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="I43" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
@@ -2878,22 +3017,25 @@
         <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>124</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
       <c r="G44">
-        <v>8</v>
+        <v>90</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2904,22 +3046,25 @@
         <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>127</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G45">
         <v>90</v>
       </c>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
       <c r="I45" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2930,22 +3075,25 @@
         <v>129</v>
       </c>
       <c r="C46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46">
-        <v>90</v>
+        <v>8</v>
+      </c>
+      <c r="H46">
+        <v>10</v>
       </c>
       <c r="I46" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -2956,22 +3104,22 @@
         <v>132</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47">
-        <v>8</v>
-      </c>
-      <c r="I47" t="s">
-        <v>309</v>
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -2982,19 +3130,25 @@
         <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -3005,22 +3159,22 @@
         <v>138</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>90</v>
-      </c>
-      <c r="I49" t="s">
-        <v>310</v>
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
@@ -3031,19 +3185,22 @@
         <v>141</v>
       </c>
       <c r="C50" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
       <c r="G50">
         <v>0</v>
+      </c>
+      <c r="H50">
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -3054,19 +3211,22 @@
         <v>144</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>145</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F51">
         <v>1</v>
       </c>
       <c r="G51">
         <v>0</v>
+      </c>
+      <c r="H51">
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
@@ -3077,19 +3237,25 @@
         <v>147</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F52">
         <v>1</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>85</v>
+      </c>
+      <c r="H52" s="4">
+        <v>0</v>
+      </c>
+      <c r="I52" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -3097,25 +3263,25 @@
         <v>149</v>
       </c>
       <c r="B53" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" t="s">
         <v>150</v>
-      </c>
-      <c r="C53" t="s">
-        <v>90</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G53">
-        <v>85</v>
-      </c>
-      <c r="I53" t="s">
-        <v>311</v>
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -3123,163 +3289,184 @@
         <v>152</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>277</v>
+        <v>309</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <v>0</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>158</v>
+        <v>274</v>
       </c>
       <c r="F55">
         <v>1</v>
       </c>
       <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55" s="4">
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C56" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F56">
+        <v>17</v>
+      </c>
+      <c r="G56">
         <v>1</v>
       </c>
-      <c r="G56">
-        <v>4</v>
-      </c>
-      <c r="I56" t="s">
-        <v>280</v>
+      <c r="H56">
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="F57">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>6</v>
+      </c>
+      <c r="I57" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C58" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F58">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G58">
         <v>0</v>
       </c>
-      <c r="I58" t="s">
-        <v>279</v>
+      <c r="H58">
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="F59">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G59">
         <v>0</v>
+      </c>
+      <c r="H59">
+        <v>6</v>
+      </c>
+      <c r="I59" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C60" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -3287,48 +3474,54 @@
       <c r="G60">
         <v>0</v>
       </c>
-      <c r="I60" t="s">
-        <v>279</v>
+      <c r="H60">
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C61" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G61">
         <v>0</v>
+      </c>
+      <c r="H61">
+        <v>3</v>
+      </c>
+      <c r="I61" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B62" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>288</v>
+        <v>308</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -3336,74 +3529,83 @@
       <c r="G62">
         <v>0</v>
       </c>
-      <c r="I62" t="s">
-        <v>279</v>
+      <c r="H62">
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>190</v>
+        <v>285</v>
       </c>
       <c r="F63">
         <v>1</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="H63" s="4">
+        <v>0</v>
+      </c>
+      <c r="I63" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F64">
         <v>1</v>
       </c>
       <c r="G64">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>2</v>
       </c>
       <c r="I64" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -3411,25 +3613,25 @@
       <c r="G65">
         <v>0</v>
       </c>
-      <c r="I65" t="s">
-        <v>279</v>
+      <c r="H65">
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -3437,31 +3639,19 @@
       <c r="G66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>203</v>
-      </c>
-      <c r="B67" t="s">
-        <v>204</v>
-      </c>
-      <c r="C67" t="s">
-        <v>205</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="I67" t="s">
-        <v>279</v>
+      <c r="H66">
+        <v>3</v>
+      </c>
+      <c r="I66" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G68" t="s">
+        <v>312</v>
+      </c>
+      <c r="H68" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>